<commit_message>
(v2.1.1.9193) new antimicrobials for screening
</commit_message>
<xml_diff>
--- a/data-raw/wisca.xlsx
+++ b/data-raw/wisca.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msberends/Unishare/Git/AMR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DD8170-1047-B244-8DB6-C76AF0D9E6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB98F1D6-23D5-3F44-8BF4-5C270FBB973E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="860" windowWidth="26440" windowHeight="21400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10860" yWindow="4360" windowWidth="29640" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>ward</t>
   </si>
@@ -37,352 +37,50 @@
     <t>Clinical</t>
   </si>
   <si>
-    <t>75.4% (64.3-85.7%)</t>
-  </si>
-  <si>
-    <t>98% (94.3-99.8%)</t>
-  </si>
-  <si>
-    <t>92.2% (82-98.2%)</t>
+    <t>73.4% (55.1-88.3%)</t>
+  </si>
+  <si>
+    <t>97.6% (92.6-99.8%)</t>
+  </si>
+  <si>
+    <t>92.1% (81.3-98.3%)</t>
   </si>
   <si>
     <t>ICU</t>
   </si>
   <si>
-    <t>89.4% (79.6-95.7%)</t>
-  </si>
-  <si>
-    <t>97.1% (90.3-99.8%)</t>
-  </si>
-  <si>
-    <t>94.7% (84.8-99.3%)</t>
+    <t>55.2% (36.8-80.3%)</t>
+  </si>
+  <si>
+    <t>95.6% (86.1-99.7%)</t>
+  </si>
+  <si>
+    <t>88.6% (70.2-98.5%)</t>
   </si>
   <si>
     <t>Outpatient</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>93.2% (79.6-99.4%)</t>
-  </si>
-  <si>
-    <t>94.3% (79.4-99.9%)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">library(AMR)   </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FF408080"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t># 2.1.1.9156</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">library(dplyr) </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FF408080"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t># 1.1.4</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">w </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF666666"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t>&lt;-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> example_isolates </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF666666"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t>%&gt;%</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">  filter_first_isolate(method </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF666666"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFBA2121"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t>"e"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">, episode_days </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF666666"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF666666"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t>14</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF666666"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t>%&gt;%</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">  top_n_microorganisms(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF666666"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF666666"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t>%&gt;%</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">  group_by(ward) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF666666"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t>%&gt;%</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">  wisca(antibiotics </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF666666"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> c(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFBA2121"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t>"TZP"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFBA2121"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t>"TZP+GEN"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFBA2121"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t>"TZP+TOB"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="1"/>
-      </rPr>
-      <t>))</t>
-    </r>
-  </si>
-  <si>
-    <t>w</t>
-  </si>
-  <si>
-    <t>retrieve_wisca_parameters(w)</t>
+    <t>63.7% (35.7-89.8%)</t>
+  </si>
+  <si>
+    <t>90.9% (71.2-99.5%)</t>
+  </si>
+  <si>
+    <t>73.7% (38.4-96.6%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Source Sans Pro"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Courier New"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color rgb="FF408080"/>
-      <name val="Courier New"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF666666"/>
-      <name val="Courier New"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFBA2121"/>
-      <name val="Courier New"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -405,12 +103,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -758,11 +455,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -828,57 +525,6 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>